<commit_message>
attempt fix lab3 1
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4B3BAD0-90C6-48DA-912A-92AD61E82147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0774B9FC-F7AF-4484-99E7-B286968686E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,13 +162,13 @@
     <t>Ершов</t>
   </si>
   <si>
+    <t>Мохамед</t>
+  </si>
+  <si>
     <t>Куропаткин 1</t>
   </si>
   <si>
     <t>Куропаткин 2</t>
-  </si>
-  <si>
-    <t>Куропаткин 3</t>
   </si>
   <si>
     <t>общая сумма графы “Итого”, руб</t>
@@ -231,17 +231,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -250,7 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -567,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,40 +587,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="9">
+      <c r="A1" s="8">
         <v>42</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -629,15 +628,15 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>70</f>
         <v>70</v>
       </c>
       <c r="E2" s="1">
-        <f>1.1 * $A$1 * IF(B2 &lt;= 8*4, 1, 0.5)</f>
+        <f>1.1 *$A$1 * IF(B2 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F2" s="1">
@@ -671,19 +670,19 @@
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <f>D2 - 0.5</f>
         <v>69.5</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E37" si="0">1.1 * $A$1 * IF(B3 &lt;= 8*4, 1, 0.5)</f>
+        <f>1.1 *$A$1 * IF(B3 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F37" si="1">D3 * E3</f>
+        <f t="shared" ref="F3:F37" si="0">D3 * E3</f>
         <v>3210.9</v>
       </c>
       <c r="G3" s="3">
@@ -695,1231 +694,1231 @@
         <v>44806</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I37" si="2">IF(H3 &lt; G3, 0, H3 - G3)</f>
+        <f>IF(H3 &lt; G3, 0, H3 - G3)</f>
         <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K37" si="3">I3*J3</f>
+        <f t="shared" ref="K3:K37" si="1">I3*J3</f>
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L38" si="4">F3+K3</f>
+        <f t="shared" ref="L3:L38" si="2">F3+K3</f>
         <v>3210.9</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B7" si="5">B3+1</f>
+        <f t="shared" ref="B4:B7" si="3">B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7">
-        <f t="shared" ref="D4:D37" si="6">D3 - 0.5</f>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D37" si="4">D3 - 0.5</f>
         <v>69</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B4 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3187.8</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G37" si="7">$G$2</f>
+        <f t="shared" ref="G4:G37" si="5">$G$2</f>
         <v>44813</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H37" si="8">H3 + 1</f>
+        <f t="shared" ref="H4:H37" si="6">H3 + 1</f>
         <v>44807</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I3:I37" si="7">IF(H4 &lt; G4, 0, H4 - G4)</f>
         <v>0</v>
       </c>
       <c r="J4" s="1">
         <v>10</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3187.8</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75">
       <c r="B5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7">
-        <f t="shared" si="6"/>
+      <c r="D5" s="6">
+        <f t="shared" si="4"/>
         <v>68.5</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B5 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3164.7000000000003</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44808</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J5" s="1">
         <v>10</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3164.7000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75">
       <c r="B6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7">
-        <f t="shared" si="6"/>
+      <c r="D6" s="6">
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B6 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3141.6000000000004</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44809</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
         <v>10</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3141.6000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75">
       <c r="B7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7">
-        <f t="shared" si="6"/>
+      <c r="D7" s="6">
+        <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B7 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3118.5</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44810</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J7" s="1">
         <v>10</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3118.5</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75">
       <c r="B8" s="2">
-        <f t="shared" ref="B6:B37" si="9">B7+1</f>
+        <f t="shared" ref="B6:B37" si="8">B7+1</f>
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="7">
-        <f t="shared" si="6"/>
+      <c r="D8" s="6">
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B8 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3095.4</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44811</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J8" s="1">
         <v>10</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3095.4</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75">
       <c r="B9" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7">
-        <f t="shared" si="6"/>
+      <c r="D9" s="6">
+        <f t="shared" si="4"/>
         <v>66.5</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B9 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3072.3</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44812</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J9" s="1">
         <v>10</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3072.3</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75">
       <c r="B10" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="7">
-        <f t="shared" si="6"/>
+      <c r="D10" s="6">
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B10 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3049.2000000000003</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J10" s="1">
         <v>10</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3049.2000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75">
       <c r="B11" s="2">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="C11" s="7" t="s">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="7">
-        <f t="shared" si="6"/>
+      <c r="D11" s="6">
+        <f t="shared" si="4"/>
         <v>65.5</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B11 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3026.1000000000004</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44814</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J11" s="1">
         <v>10</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3036.1000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75">
       <c r="B12" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7">
-        <f t="shared" si="6"/>
+      <c r="D12" s="6">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B12 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3003</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44815</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J12" s="1">
         <v>10</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3023</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75">
       <c r="B13" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="7">
-        <f t="shared" si="6"/>
+      <c r="D13" s="6">
+        <f t="shared" si="4"/>
         <v>64.5</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B13 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2979.9</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="J13" s="1">
         <v>10</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3009.9</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75">
       <c r="B14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="7">
-        <f t="shared" si="6"/>
+      <c r="D14" s="6">
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B14 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2956.8</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44817</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J14" s="1">
         <v>10</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2996.8</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75">
       <c r="B15" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="7">
-        <f t="shared" si="6"/>
+      <c r="D15" s="6">
+        <f t="shared" si="4"/>
         <v>63.5</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B15 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2933.7000000000003</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44818</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="J15" s="1">
         <v>10</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2983.7000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75">
       <c r="B16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="7">
-        <f t="shared" si="6"/>
+      <c r="D16" s="6">
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B16 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2910.6000000000004</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44819</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="J16" s="1">
         <v>10</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2970.6000000000004</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="15.75">
       <c r="B17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="7">
-        <f t="shared" si="6"/>
+      <c r="D17" s="6">
+        <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B17 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2887.5</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44820</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="J17" s="1">
         <v>10</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2957.5</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75">
       <c r="B18" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="7">
-        <f t="shared" si="6"/>
+      <c r="D18" s="6">
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B18 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2864.4</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44821</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2944.4</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75">
       <c r="B19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="7">
-        <f t="shared" si="6"/>
+      <c r="D19" s="6">
+        <f t="shared" si="4"/>
         <v>61.5</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B19 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2841.3</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44822</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="J19" s="1">
         <v>10</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2931.3</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75">
       <c r="B20" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="7">
-        <f t="shared" si="6"/>
+      <c r="D20" s="6">
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B20 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2818.2000000000003</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44823</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="J20" s="1">
         <v>10</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2918.2000000000003</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="15.75">
       <c r="B21" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="7">
-        <f t="shared" si="6"/>
+      <c r="D21" s="6">
+        <f t="shared" si="4"/>
         <v>60.5</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B21 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2795.1000000000004</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44824</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="J21" s="1">
         <v>10</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2905.1000000000004</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75">
       <c r="B22" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="7">
-        <f t="shared" si="6"/>
+      <c r="D22" s="6">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B22 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2772</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44825</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="J22" s="1">
         <v>10</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2892</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75">
       <c r="B23" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="7">
-        <f t="shared" si="6"/>
+      <c r="D23" s="6">
+        <f t="shared" si="4"/>
         <v>59.5</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B23 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2748.9</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44826</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="J23" s="1">
         <v>10</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2878.9</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75">
       <c r="B24" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="7">
-        <f t="shared" si="6"/>
+      <c r="D24" s="6">
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B24 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2725.8</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44827</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="J24" s="1">
         <v>10</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2865.8</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15.75">
       <c r="B25" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="7">
-        <f t="shared" si="6"/>
+      <c r="D25" s="6">
+        <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B25 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2702.7000000000003</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44828</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="J25" s="1">
         <v>10</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2852.7000000000003</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75">
       <c r="B26" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="7">
-        <f t="shared" si="6"/>
+      <c r="D26" s="6">
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B26 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2679.6000000000004</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44829</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="J26" s="1">
         <v>10</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2839.6000000000004</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="15.75">
       <c r="B27" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="7">
-        <f t="shared" si="6"/>
+      <c r="D27" s="6">
+        <f t="shared" si="4"/>
         <v>57.5</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B27 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2656.5</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44830</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="J27" s="1">
         <v>10</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>170</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2826.5</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="15.75">
       <c r="B28" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="7">
-        <f t="shared" si="6"/>
+      <c r="D28" s="6">
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B28 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2633.4</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44831</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="J28" s="1">
         <v>10</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2813.4</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="15.75">
       <c r="B29" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="7">
-        <f t="shared" si="6"/>
+      <c r="D29" s="6">
+        <f t="shared" si="4"/>
         <v>56.5</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B29 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2610.3000000000002</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44832</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="J29" s="1">
         <v>10</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>190</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2800.3</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="15.75">
       <c r="B30" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="7">
-        <f t="shared" si="6"/>
+      <c r="D30" s="6">
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B30 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2587.2000000000003</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44833</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="J30" s="1">
         <v>10</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2787.2000000000003</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="15.75">
       <c r="B31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="7">
-        <f t="shared" si="6"/>
+      <c r="D31" s="6">
+        <f t="shared" si="4"/>
         <v>55.5</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B31 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2564.1000000000004</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H31" s="3">
@@ -1927,215 +1926,215 @@
         <v>44834</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="J31" s="1">
         <v>10</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2774.1000000000004</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="15.75">
       <c r="B32" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="7">
-        <f t="shared" si="6"/>
+      <c r="D32" s="6">
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B32 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2541</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44835</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="J32" s="1">
         <v>10</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2761</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="15.75">
       <c r="B33" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="7">
-        <f t="shared" si="6"/>
+      <c r="D33" s="6">
+        <f t="shared" si="4"/>
         <v>54.5</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B33 &lt;= 8*4, 1, 0.5)</f>
         <v>46.2</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2517.9</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44836</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="J33" s="1">
         <v>10</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>230</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2747.9</v>
       </c>
     </row>
     <row r="34" spans="2:12" ht="15.75">
       <c r="B34" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="7">
-        <f t="shared" si="6"/>
+      <c r="D34" s="6">
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B34 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1247.4000000000001</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44837</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="J34" s="1">
         <v>10</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1487.4</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="15.75">
       <c r="B35" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="7">
-        <f t="shared" si="6"/>
+      <c r="D35" s="6">
+        <f t="shared" si="4"/>
         <v>53.5</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B35 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1235.8500000000001</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44838</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="J35" s="1">
         <v>10</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1485.8500000000001</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="15.75">
       <c r="B36" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="7">
-        <f t="shared" si="6"/>
+      <c r="D36" s="6">
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B36 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1224.3000000000002</v>
       </c>
       <c r="G36" s="3">
@@ -2143,66 +2142,66 @@
         <v>44813</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44839</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="J36" s="1">
         <v>10</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>260</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1484.3000000000002</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="15.75">
       <c r="B37" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="7">
-        <f t="shared" si="6"/>
+      <c r="D37" s="6">
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="0"/>
+        <f>1.1 *$A$1 * IF(B37 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1212.75</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>44813</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>44840</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="J37" s="1">
         <v>10</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1482.75</v>
       </c>
     </row>
@@ -2211,44 +2210,41 @@
     </row>
     <row r="39" spans="2:12" ht="15.75"/>
     <row r="40" spans="2:12" ht="15.75">
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <f>SUM(L2:L37)</f>
         <v>100730.7</v>
       </c>
-      <c r="D40" s="5"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="2:12" ht="15.75">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="1">
         <f>AVERAGE(D2:D37)</f>
         <v>61.25</v>
       </c>
-      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="2:12" ht="15.75">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="1">
         <f>MAX(I2:I37)</f>
         <v>27</v>
       </c>
-      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="2:12" ht="15.75">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="1">
         <f>MAX(F2:F37)</f>
         <v>3234</v>
       </c>
-      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="2:12" ht="15.75"/>
     <row r="45" spans="2:12" ht="15.75"/>
@@ -2265,6 +2261,7 @@
     <row r="56" ht="15.75"/>
     <row r="57" ht="15.75"/>
     <row r="58" ht="15.75"/>
+    <row r="59" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
attempt fix lab3 3
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0774B9FC-F7AF-4484-99E7-B286968686E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8256902-27B3-4001-8697-910CB4052642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,1691 +566,1691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
-    <col min="9" max="12" width="18.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="1" customWidth="1"/>
+    <col min="8" max="11" width="18.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="8">
+    <row r="1" spans="1:11" ht="15.75">
+      <c r="A1" s="1">
         <v>42</v>
       </c>
-      <c r="B1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="15.75">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
-      <c r="B2" s="2">
+      <c r="K2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5">
+      <c r="C3" s="5">
         <f>70</f>
         <v>70</v>
       </c>
-      <c r="E2" s="1">
-        <f>1.1 *$A$1 * IF(B2 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F2" s="1">
-        <f>D2 * E2</f>
+      <c r="D3" s="1">
+        <f>1.1 *$A$1 * IF(A3 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E3" s="1">
+        <f>C3 * D3</f>
         <v>3234</v>
       </c>
-      <c r="G2" s="3">
-        <v>44813</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="F3" s="3">
+        <v>44813</v>
+      </c>
+      <c r="G3" s="3">
         <v>44805</v>
       </c>
-      <c r="I2" s="1">
-        <f>IF(H2 &lt; G2, 0, H2 - G2)</f>
+      <c r="H3" s="1">
+        <f>IF(G3 &lt; F3, 0, G3 - F3)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1">
-        <f>I2*J2</f>
+      <c r="I3" s="1">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <f>H3*I3</f>
         <v>0</v>
       </c>
-      <c r="L2" s="1">
-        <f>F2+K2</f>
+      <c r="K3" s="1">
+        <f>E3+J3</f>
         <v>3234</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
-      <c r="B3" s="2">
-        <f>B2+1</f>
+    <row r="4" spans="1:11" ht="15.75">
+      <c r="A4" s="2">
+        <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6">
-        <f>D2 - 0.5</f>
+      <c r="C4" s="6">
+        <f>C3 - 0.5</f>
         <v>69.5</v>
       </c>
-      <c r="E3" s="1">
-        <f>1.1 *$A$1 * IF(B3 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F37" si="0">D3 * E3</f>
+      <c r="D4" s="1">
+        <f>1.1 *$A$1 * IF(A4 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E38" si="0">C4 * D4</f>
         <v>3210.9</v>
       </c>
-      <c r="G3" s="3">
-        <f>$G$2</f>
-        <v>44813</v>
-      </c>
-      <c r="H3" s="3">
-        <f>H2 + 1</f>
+      <c r="F4" s="3">
+        <f>$F$3</f>
+        <v>44813</v>
+      </c>
+      <c r="G4" s="3">
+        <f>G3 + 1</f>
         <v>44806</v>
       </c>
-      <c r="I3" s="1">
-        <f>IF(H3 &lt; G3, 0, H3 - G3)</f>
+      <c r="H4" s="1">
+        <f>IF(G4 &lt; F4, 0, G4 - F4)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="1">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K37" si="1">I3*J3</f>
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J38" si="1">H4*I4</f>
         <v>0</v>
       </c>
-      <c r="L3" s="1">
-        <f t="shared" ref="L3:L38" si="2">F3+K3</f>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K39" si="2">E4+J4</f>
         <v>3210.9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75">
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:B7" si="3">B3+1</f>
+    <row r="5" spans="1:11" ht="15.75">
+      <c r="A5" s="2">
+        <f t="shared" ref="A5:A8" si="3">A4+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" ref="D4:D37" si="4">D3 - 0.5</f>
+      <c r="C5" s="6">
+        <f t="shared" ref="C5:C38" si="4">C4 - 0.5</f>
         <v>69</v>
       </c>
-      <c r="E4" s="1">
-        <f>1.1 *$A$1 * IF(B4 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D5" s="1">
+        <f>1.1 *$A$1 * IF(A5 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>3187.8</v>
       </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:G37" si="5">$G$2</f>
-        <v>44813</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" ref="H4:H37" si="6">H3 + 1</f>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F38" si="5">$F$3</f>
+        <v>44813</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:G38" si="6">G4 + 1</f>
         <v>44807</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" ref="I3:I37" si="7">IF(H4 &lt; G4, 0, H4 - G4)</f>
+      <c r="H5" s="1">
+        <f t="shared" ref="H4:H38" si="7">IF(G5 &lt; F5, 0, G5 - F5)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="1">
-        <v>10</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="I5" s="1">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L4" s="1">
+      <c r="K5" s="1">
         <f t="shared" si="2"/>
         <v>3187.8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
-      <c r="B5" s="2">
+    <row r="6" spans="1:11" ht="15.75">
+      <c r="A6" s="2">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="C6" s="6">
         <f t="shared" si="4"/>
         <v>68.5</v>
       </c>
-      <c r="E5" s="1">
-        <f>1.1 *$A$1 * IF(B5 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="D6" s="1">
+        <f>1.1 *$A$1 * IF(A6 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>3164.7000000000003</v>
       </c>
-      <c r="G5" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="F6" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G6" s="3">
         <f t="shared" si="6"/>
         <v>44808</v>
       </c>
-      <c r="I5" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J5" s="1">
-        <v>10</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="I6" s="1">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="1">
+      <c r="K6" s="1">
         <f t="shared" si="2"/>
         <v>3164.7000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
-      <c r="B6" s="2">
+    <row r="7" spans="1:11" ht="15.75">
+      <c r="A7" s="2">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6">
+      <c r="C7" s="6">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="E6" s="1">
-        <f>1.1 *$A$1 * IF(B6 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="D7" s="1">
+        <f>1.1 *$A$1 * IF(A7 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>3141.6000000000004</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="F7" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G7" s="3">
         <f t="shared" si="6"/>
         <v>44809</v>
       </c>
-      <c r="I6" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J6" s="1">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="1">
+      <c r="K7" s="1">
         <f t="shared" si="2"/>
         <v>3141.6000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
-      <c r="B7" s="2">
+    <row r="8" spans="1:11" ht="15.75">
+      <c r="A8" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6">
+      <c r="C8" s="6">
         <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
-      <c r="E7" s="1">
-        <f>1.1 *$A$1 * IF(B7 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="D8" s="1">
+        <f>1.1 *$A$1 * IF(A8 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>3118.5</v>
       </c>
-      <c r="G7" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="F8" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G8" s="3">
         <f t="shared" si="6"/>
         <v>44810</v>
       </c>
-      <c r="I7" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J7" s="1">
-        <v>10</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="I8" s="1">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="1">
+      <c r="K8" s="1">
         <f t="shared" si="2"/>
         <v>3118.5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
-      <c r="B8" s="2">
-        <f t="shared" ref="B6:B37" si="8">B7+1</f>
+    <row r="9" spans="1:11" ht="15.75">
+      <c r="A9" s="2">
+        <f t="shared" ref="A7:A38" si="8">A8+1</f>
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6">
+      <c r="C9" s="6">
         <f t="shared" si="4"/>
         <v>67</v>
       </c>
-      <c r="E8" s="1">
-        <f>1.1 *$A$1 * IF(B8 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="D9" s="1">
+        <f>1.1 *$A$1 * IF(A9 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>3095.4</v>
       </c>
-      <c r="G8" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="F9" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G9" s="3">
         <f t="shared" si="6"/>
         <v>44811</v>
       </c>
-      <c r="I8" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J8" s="1">
-        <v>10</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="I9" s="1">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="1">
+      <c r="K9" s="1">
         <f t="shared" si="2"/>
         <v>3095.4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
-      <c r="B9" s="2">
+    <row r="10" spans="1:11" ht="15.75">
+      <c r="A10" s="2">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="6">
+      <c r="C10" s="6">
         <f t="shared" si="4"/>
         <v>66.5</v>
       </c>
-      <c r="E9" s="1">
-        <f>1.1 *$A$1 * IF(B9 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="D10" s="1">
+        <f>1.1 *$A$1 * IF(A10 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>3072.3</v>
       </c>
-      <c r="G9" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="F10" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G10" s="3">
         <f t="shared" si="6"/>
         <v>44812</v>
       </c>
-      <c r="I9" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J9" s="1">
-        <v>10</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="I10" s="1">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="1">
+      <c r="K10" s="1">
         <f t="shared" si="2"/>
         <v>3072.3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
-      <c r="B10" s="2">
+    <row r="11" spans="1:11" ht="15.75">
+      <c r="A11" s="2">
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6">
+      <c r="C11" s="6">
         <f t="shared" si="4"/>
         <v>66</v>
       </c>
-      <c r="E10" s="1">
-        <f>1.1 *$A$1 * IF(B10 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="D11" s="1">
+        <f>1.1 *$A$1 * IF(A11 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>3049.2000000000003</v>
       </c>
-      <c r="G10" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="6"/>
-        <v>44813</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="F11" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="6"/>
+        <v>44813</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J10" s="1">
-        <v>10</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="I11" s="1">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="1">
+      <c r="K11" s="1">
         <f t="shared" si="2"/>
         <v>3049.2000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
-      <c r="B11" s="2">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    <row r="12" spans="1:11" ht="15.75">
+      <c r="A12" s="2">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="6">
+      <c r="C12" s="6">
         <f t="shared" si="4"/>
         <v>65.5</v>
       </c>
-      <c r="E11" s="1">
-        <f>1.1 *$A$1 * IF(B11 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="D12" s="1">
+        <f>1.1 *$A$1 * IF(A12 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>3026.1000000000004</v>
       </c>
-      <c r="G11" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="F12" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G12" s="3">
         <f t="shared" si="6"/>
         <v>44814</v>
       </c>
-      <c r="I11" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="J11" s="1">
-        <v>10</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="I12" s="1">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="1">
         <f t="shared" si="2"/>
         <v>3036.1000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
-      <c r="B12" s="2">
+    <row r="13" spans="1:11" ht="15.75">
+      <c r="A13" s="2">
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="6">
+      <c r="C13" s="6">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="E12" s="1">
-        <f>1.1 *$A$1 * IF(B12 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="D13" s="1">
+        <f>1.1 *$A$1 * IF(A13 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>3003</v>
       </c>
-      <c r="G12" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="F13" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G13" s="3">
         <f t="shared" si="6"/>
         <v>44815</v>
       </c>
-      <c r="I12" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="J12" s="1">
-        <v>10</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="I13" s="1">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="L12" s="1">
+      <c r="K13" s="1">
         <f t="shared" si="2"/>
         <v>3023</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
-      <c r="B13" s="2">
+    <row r="14" spans="1:11" ht="15.75">
+      <c r="A14" s="2">
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="6">
+      <c r="C14" s="6">
         <f t="shared" si="4"/>
         <v>64.5</v>
       </c>
-      <c r="E13" s="1">
-        <f>1.1 *$A$1 * IF(B13 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="D14" s="1">
+        <f>1.1 *$A$1 * IF(A14 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>2979.9</v>
       </c>
-      <c r="G13" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="F14" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G14" s="3">
         <f t="shared" si="6"/>
         <v>44816</v>
       </c>
-      <c r="I13" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="J13" s="1">
-        <v>10</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="I14" s="1">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="L13" s="1">
+      <c r="K14" s="1">
         <f t="shared" si="2"/>
         <v>3009.9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
-      <c r="B14" s="2">
+    <row r="15" spans="1:11" ht="15.75">
+      <c r="A15" s="2">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="6">
+      <c r="C15" s="6">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="E14" s="1">
-        <f>1.1 *$A$1 * IF(B14 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="D15" s="1">
+        <f>1.1 *$A$1 * IF(A15 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>2956.8</v>
       </c>
-      <c r="G14" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="F15" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G15" s="3">
         <f t="shared" si="6"/>
         <v>44817</v>
       </c>
-      <c r="I14" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="J14" s="1">
-        <v>10</v>
-      </c>
-      <c r="K14" s="1">
+      <c r="I15" s="1">
+        <v>10</v>
+      </c>
+      <c r="J15" s="1">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L14" s="1">
+      <c r="K15" s="1">
         <f t="shared" si="2"/>
         <v>2996.8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
-      <c r="B15" s="2">
+    <row r="16" spans="1:11" ht="15.75">
+      <c r="A16" s="2">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="6">
+      <c r="C16" s="6">
         <f t="shared" si="4"/>
         <v>63.5</v>
       </c>
-      <c r="E15" s="1">
-        <f>1.1 *$A$1 * IF(B15 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="D16" s="1">
+        <f>1.1 *$A$1 * IF(A16 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>2933.7000000000003</v>
       </c>
-      <c r="G15" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="F16" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G16" s="3">
         <f t="shared" si="6"/>
         <v>44818</v>
       </c>
-      <c r="I15" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="J15" s="1">
-        <v>10</v>
-      </c>
-      <c r="K15" s="1">
+      <c r="I16" s="1">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="L15" s="1">
+      <c r="K16" s="1">
         <f t="shared" si="2"/>
         <v>2983.7000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="B16" s="2">
+    <row r="17" spans="1:11" ht="15.75">
+      <c r="A17" s="2">
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="6">
+      <c r="C17" s="6">
         <f t="shared" si="4"/>
         <v>63</v>
       </c>
-      <c r="E16" s="1">
-        <f>1.1 *$A$1 * IF(B16 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="D17" s="1">
+        <f>1.1 *$A$1 * IF(A17 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>2910.6000000000004</v>
       </c>
-      <c r="G16" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="F17" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G17" s="3">
         <f t="shared" si="6"/>
         <v>44819</v>
       </c>
-      <c r="I16" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="J16" s="1">
-        <v>10</v>
-      </c>
-      <c r="K16" s="1">
+      <c r="I17" s="1">
+        <v>10</v>
+      </c>
+      <c r="J17" s="1">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="L16" s="1">
+      <c r="K17" s="1">
         <f t="shared" si="2"/>
         <v>2970.6000000000004</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.75">
-      <c r="B17" s="2">
+    <row r="18" spans="1:11" ht="15.75">
+      <c r="A18" s="2">
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="6">
+      <c r="C18" s="6">
         <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
-      <c r="E17" s="1">
-        <f>1.1 *$A$1 * IF(B17 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="D18" s="1">
+        <f>1.1 *$A$1 * IF(A18 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>2887.5</v>
       </c>
-      <c r="G17" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="F18" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G18" s="3">
         <f t="shared" si="6"/>
         <v>44820</v>
       </c>
-      <c r="I17" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="J17" s="1">
-        <v>10</v>
-      </c>
-      <c r="K17" s="1">
+      <c r="I18" s="1">
+        <v>10</v>
+      </c>
+      <c r="J18" s="1">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="L17" s="1">
+      <c r="K18" s="1">
         <f t="shared" si="2"/>
         <v>2957.5</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.75">
-      <c r="B18" s="2">
+    <row r="19" spans="1:11" ht="15.75">
+      <c r="A19" s="2">
         <f t="shared" si="8"/>
         <v>17</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="6">
+      <c r="C19" s="6">
         <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="E18" s="1">
-        <f>1.1 *$A$1 * IF(B18 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="D19" s="1">
+        <f>1.1 *$A$1 * IF(A19 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>2864.4</v>
       </c>
-      <c r="G18" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="F19" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G19" s="3">
         <f t="shared" si="6"/>
         <v>44821</v>
       </c>
-      <c r="I18" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J18" s="1">
-        <v>10</v>
-      </c>
-      <c r="K18" s="1">
+      <c r="I19" s="1">
+        <v>10</v>
+      </c>
+      <c r="J19" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="L18" s="1">
+      <c r="K19" s="1">
         <f t="shared" si="2"/>
         <v>2944.4</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.75">
-      <c r="B19" s="2">
+    <row r="20" spans="1:11" ht="15.75">
+      <c r="A20" s="2">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="6">
+      <c r="C20" s="6">
         <f t="shared" si="4"/>
         <v>61.5</v>
       </c>
-      <c r="E19" s="1">
-        <f>1.1 *$A$1 * IF(B19 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="D20" s="1">
+        <f>1.1 *$A$1 * IF(A20 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>2841.3</v>
       </c>
-      <c r="G19" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="F20" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G20" s="3">
         <f t="shared" si="6"/>
         <v>44822</v>
       </c>
-      <c r="I19" s="1">
+      <c r="H20" s="1">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="J19" s="1">
-        <v>10</v>
-      </c>
-      <c r="K19" s="1">
+      <c r="I20" s="1">
+        <v>10</v>
+      </c>
+      <c r="J20" s="1">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="L19" s="1">
+      <c r="K20" s="1">
         <f t="shared" si="2"/>
         <v>2931.3</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15.75">
-      <c r="B20" s="2">
+    <row r="21" spans="1:11" ht="15.75">
+      <c r="A21" s="2">
         <f t="shared" si="8"/>
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="6">
+      <c r="C21" s="6">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="E20" s="1">
-        <f>1.1 *$A$1 * IF(B20 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="D21" s="1">
+        <f>1.1 *$A$1 * IF(A21 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>2818.2000000000003</v>
       </c>
-      <c r="G20" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="F21" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G21" s="3">
         <f t="shared" si="6"/>
         <v>44823</v>
       </c>
-      <c r="I20" s="1">
-        <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="J20" s="1">
-        <v>10</v>
-      </c>
-      <c r="K20" s="1">
+      <c r="H21" s="1">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I21" s="1">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="L20" s="1">
+      <c r="K21" s="1">
         <f t="shared" si="2"/>
         <v>2918.2000000000003</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15.75">
-      <c r="B21" s="2">
+    <row r="22" spans="1:11" ht="15.75">
+      <c r="A22" s="2">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="6">
+      <c r="C22" s="6">
         <f t="shared" si="4"/>
         <v>60.5</v>
       </c>
-      <c r="E21" s="1">
-        <f>1.1 *$A$1 * IF(B21 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="D22" s="1">
+        <f>1.1 *$A$1 * IF(A22 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>2795.1000000000004</v>
       </c>
-      <c r="G21" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="F22" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G22" s="3">
         <f t="shared" si="6"/>
         <v>44824</v>
       </c>
-      <c r="I21" s="1">
+      <c r="H22" s="1">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="J21" s="1">
-        <v>10</v>
-      </c>
-      <c r="K21" s="1">
+      <c r="I22" s="1">
+        <v>10</v>
+      </c>
+      <c r="J22" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="L21" s="1">
+      <c r="K22" s="1">
         <f t="shared" si="2"/>
         <v>2905.1000000000004</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.75">
-      <c r="B22" s="2">
+    <row r="23" spans="1:11" ht="15.75">
+      <c r="A23" s="2">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="6">
+      <c r="C23" s="6">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="E22" s="1">
-        <f>1.1 *$A$1 * IF(B22 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="D23" s="1">
+        <f>1.1 *$A$1 * IF(A23 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>2772</v>
       </c>
-      <c r="G22" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="F23" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G23" s="3">
         <f t="shared" si="6"/>
         <v>44825</v>
       </c>
-      <c r="I22" s="1">
+      <c r="H23" s="1">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="J22" s="1">
-        <v>10</v>
-      </c>
-      <c r="K22" s="1">
+      <c r="I23" s="1">
+        <v>10</v>
+      </c>
+      <c r="J23" s="1">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="L22" s="1">
+      <c r="K23" s="1">
         <f t="shared" si="2"/>
         <v>2892</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="15.75">
-      <c r="B23" s="2">
+    <row r="24" spans="1:11" ht="15.75">
+      <c r="A24" s="2">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="6">
+      <c r="C24" s="6">
         <f t="shared" si="4"/>
         <v>59.5</v>
       </c>
-      <c r="E23" s="1">
-        <f>1.1 *$A$1 * IF(B23 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F23" s="1">
+      <c r="D24" s="1">
+        <f>1.1 *$A$1 * IF(A24 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>2748.9</v>
       </c>
-      <c r="G23" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="F24" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G24" s="3">
         <f t="shared" si="6"/>
         <v>44826</v>
       </c>
-      <c r="I23" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="J23" s="1">
-        <v>10</v>
-      </c>
-      <c r="K23" s="1">
+      <c r="I24" s="1">
+        <v>10</v>
+      </c>
+      <c r="J24" s="1">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="L23" s="1">
+      <c r="K24" s="1">
         <f t="shared" si="2"/>
         <v>2878.9</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="15.75">
-      <c r="B24" s="2">
+    <row r="25" spans="1:11" ht="15.75">
+      <c r="A25" s="2">
         <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="6">
+      <c r="C25" s="6">
         <f t="shared" si="4"/>
         <v>59</v>
       </c>
-      <c r="E24" s="1">
-        <f>1.1 *$A$1 * IF(B24 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="D25" s="1">
+        <f>1.1 *$A$1 * IF(A25 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>2725.8</v>
       </c>
-      <c r="G24" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H24" s="3">
+      <c r="F25" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G25" s="3">
         <f t="shared" si="6"/>
         <v>44827</v>
       </c>
-      <c r="I24" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="J24" s="1">
-        <v>10</v>
-      </c>
-      <c r="K24" s="1">
+      <c r="I25" s="1">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="L24" s="1">
+      <c r="K25" s="1">
         <f t="shared" si="2"/>
         <v>2865.8</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="15.75">
-      <c r="B25" s="2">
+    <row r="26" spans="1:11" ht="15.75">
+      <c r="A26" s="2">
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="6">
+      <c r="C26" s="6">
         <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
-      <c r="E25" s="1">
-        <f>1.1 *$A$1 * IF(B25 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="D26" s="1">
+        <f>1.1 *$A$1 * IF(A26 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>2702.7000000000003</v>
       </c>
-      <c r="G25" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H25" s="3">
+      <c r="F26" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G26" s="3">
         <f t="shared" si="6"/>
         <v>44828</v>
       </c>
-      <c r="I25" s="1">
+      <c r="H26" s="1">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="J25" s="1">
-        <v>10</v>
-      </c>
-      <c r="K25" s="1">
+      <c r="I26" s="1">
+        <v>10</v>
+      </c>
+      <c r="J26" s="1">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="L25" s="1">
+      <c r="K26" s="1">
         <f t="shared" si="2"/>
         <v>2852.7000000000003</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15.75">
-      <c r="B26" s="2">
+    <row r="27" spans="1:11" ht="15.75">
+      <c r="A27" s="2">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="6">
+      <c r="C27" s="6">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="E26" s="1">
-        <f>1.1 *$A$1 * IF(B26 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="D27" s="1">
+        <f>1.1 *$A$1 * IF(A27 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
         <v>2679.6000000000004</v>
       </c>
-      <c r="G26" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="F27" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G27" s="3">
         <f t="shared" si="6"/>
         <v>44829</v>
       </c>
-      <c r="I26" s="1">
+      <c r="H27" s="1">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="J26" s="1">
-        <v>10</v>
-      </c>
-      <c r="K26" s="1">
+      <c r="I27" s="1">
+        <v>10</v>
+      </c>
+      <c r="J27" s="1">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="L26" s="1">
+      <c r="K27" s="1">
         <f t="shared" si="2"/>
         <v>2839.6000000000004</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="15.75">
-      <c r="B27" s="2">
+    <row r="28" spans="1:11" ht="15.75">
+      <c r="A28" s="2">
         <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="6">
+      <c r="C28" s="6">
         <f t="shared" si="4"/>
         <v>57.5</v>
       </c>
-      <c r="E27" s="1">
-        <f>1.1 *$A$1 * IF(B27 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="D28" s="1">
+        <f>1.1 *$A$1 * IF(A28 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E28" s="1">
         <f t="shared" si="0"/>
         <v>2656.5</v>
       </c>
-      <c r="G27" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H27" s="3">
+      <c r="F28" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G28" s="3">
         <f t="shared" si="6"/>
         <v>44830</v>
       </c>
-      <c r="I27" s="1">
+      <c r="H28" s="1">
         <f t="shared" si="7"/>
         <v>17</v>
       </c>
-      <c r="J27" s="1">
-        <v>10</v>
-      </c>
-      <c r="K27" s="1">
+      <c r="I28" s="1">
+        <v>10</v>
+      </c>
+      <c r="J28" s="1">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="L27" s="1">
+      <c r="K28" s="1">
         <f t="shared" si="2"/>
         <v>2826.5</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75">
-      <c r="B28" s="2">
+    <row r="29" spans="1:11" ht="15.75">
+      <c r="A29" s="2">
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="6">
+      <c r="C29" s="6">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="E28" s="1">
-        <f>1.1 *$A$1 * IF(B28 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="D29" s="1">
+        <f>1.1 *$A$1 * IF(A29 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E29" s="1">
         <f t="shared" si="0"/>
         <v>2633.4</v>
       </c>
-      <c r="G28" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H28" s="3">
+      <c r="F29" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G29" s="3">
         <f t="shared" si="6"/>
         <v>44831</v>
       </c>
-      <c r="I28" s="1">
+      <c r="H29" s="1">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="J28" s="1">
-        <v>10</v>
-      </c>
-      <c r="K28" s="1">
+      <c r="I29" s="1">
+        <v>10</v>
+      </c>
+      <c r="J29" s="1">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="L28" s="1">
+      <c r="K29" s="1">
         <f t="shared" si="2"/>
         <v>2813.4</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="15.75">
-      <c r="B29" s="2">
+    <row r="30" spans="1:11" ht="15.75">
+      <c r="A30" s="2">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="6">
+      <c r="C30" s="6">
         <f t="shared" si="4"/>
         <v>56.5</v>
       </c>
-      <c r="E29" s="1">
-        <f>1.1 *$A$1 * IF(B29 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="D30" s="1">
+        <f>1.1 *$A$1 * IF(A30 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>2610.3000000000002</v>
       </c>
-      <c r="G29" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H29" s="3">
+      <c r="F30" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G30" s="3">
         <f t="shared" si="6"/>
         <v>44832</v>
       </c>
-      <c r="I29" s="1">
+      <c r="H30" s="1">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="J29" s="1">
-        <v>10</v>
-      </c>
-      <c r="K29" s="1">
+      <c r="I30" s="1">
+        <v>10</v>
+      </c>
+      <c r="J30" s="1">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="L29" s="1">
+      <c r="K30" s="1">
         <f t="shared" si="2"/>
         <v>2800.3</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15.75">
-      <c r="B30" s="2">
+    <row r="31" spans="1:11" ht="15.75">
+      <c r="A31" s="2">
         <f t="shared" si="8"/>
         <v>29</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="6">
+      <c r="C31" s="6">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="E30" s="1">
-        <f>1.1 *$A$1 * IF(B30 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="D31" s="1">
+        <f>1.1 *$A$1 * IF(A31 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E31" s="1">
         <f t="shared" si="0"/>
         <v>2587.2000000000003</v>
       </c>
-      <c r="G30" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H30" s="3">
+      <c r="F31" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G31" s="3">
         <f t="shared" si="6"/>
         <v>44833</v>
       </c>
-      <c r="I30" s="1">
+      <c r="H31" s="1">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="J30" s="1">
-        <v>10</v>
-      </c>
-      <c r="K30" s="1">
+      <c r="I31" s="1">
+        <v>10</v>
+      </c>
+      <c r="J31" s="1">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="L30" s="1">
+      <c r="K31" s="1">
         <f t="shared" si="2"/>
         <v>2787.2000000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15.75">
-      <c r="B31" s="2">
+    <row r="32" spans="1:11" ht="15.75">
+      <c r="A32" s="2">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="6">
+      <c r="C32" s="6">
         <f t="shared" si="4"/>
         <v>55.5</v>
       </c>
-      <c r="E31" s="1">
-        <f>1.1 *$A$1 * IF(B31 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="D32" s="1">
+        <f>1.1 *$A$1 * IF(A32 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E32" s="1">
         <f t="shared" si="0"/>
         <v>2564.1000000000004</v>
       </c>
-      <c r="G31" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H31" s="3">
-        <f>H30 + 1</f>
+      <c r="F32" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G32" s="3">
+        <f>G31 + 1</f>
         <v>44834</v>
       </c>
-      <c r="I31" s="1">
+      <c r="H32" s="1">
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="J31" s="1">
-        <v>10</v>
-      </c>
-      <c r="K31" s="1">
+      <c r="I32" s="1">
+        <v>10</v>
+      </c>
+      <c r="J32" s="1">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="L31" s="1">
+      <c r="K32" s="1">
         <f t="shared" si="2"/>
         <v>2774.1000000000004</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15.75">
-      <c r="B32" s="2">
+    <row r="33" spans="1:11" ht="15.75">
+      <c r="A33" s="2">
         <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="6">
+      <c r="C33" s="6">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="E32" s="1">
-        <f>1.1 *$A$1 * IF(B32 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F32" s="1">
+      <c r="D33" s="1">
+        <f>1.1 *$A$1 * IF(A33 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E33" s="1">
         <f t="shared" si="0"/>
         <v>2541</v>
       </c>
-      <c r="G32" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H32" s="3">
+      <c r="F33" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G33" s="3">
         <f t="shared" si="6"/>
         <v>44835</v>
       </c>
-      <c r="I32" s="1">
+      <c r="H33" s="1">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="J32" s="1">
-        <v>10</v>
-      </c>
-      <c r="K32" s="1">
+      <c r="I33" s="1">
+        <v>10</v>
+      </c>
+      <c r="J33" s="1">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="L32" s="1">
+      <c r="K33" s="1">
         <f t="shared" si="2"/>
         <v>2761</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="15.75">
-      <c r="B33" s="2">
+    <row r="34" spans="1:11" ht="15.75">
+      <c r="A34" s="2">
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="6">
+      <c r="C34" s="6">
         <f t="shared" si="4"/>
         <v>54.5</v>
       </c>
-      <c r="E33" s="1">
-        <f>1.1 *$A$1 * IF(B33 &lt;= 8*4, 1, 0.5)</f>
-        <v>46.2</v>
-      </c>
-      <c r="F33" s="1">
+      <c r="D34" s="1">
+        <f>1.1 *$A$1 * IF(A34 &lt;= 8*4, 1, 0.5)</f>
+        <v>46.2</v>
+      </c>
+      <c r="E34" s="1">
         <f t="shared" si="0"/>
         <v>2517.9</v>
       </c>
-      <c r="G33" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H33" s="3">
+      <c r="F34" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G34" s="3">
         <f t="shared" si="6"/>
         <v>44836</v>
       </c>
-      <c r="I33" s="1">
+      <c r="H34" s="1">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="J33" s="1">
-        <v>10</v>
-      </c>
-      <c r="K33" s="1">
+      <c r="I34" s="1">
+        <v>10</v>
+      </c>
+      <c r="J34" s="1">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
-      <c r="L33" s="1">
+      <c r="K34" s="1">
         <f t="shared" si="2"/>
         <v>2747.9</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="15.75">
-      <c r="B34" s="2">
+    <row r="35" spans="1:11" ht="15.75">
+      <c r="A35" s="2">
         <f t="shared" si="8"/>
         <v>33</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="6">
+      <c r="C35" s="6">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="E34" s="1">
-        <f>1.1 *$A$1 * IF(B34 &lt;= 8*4, 1, 0.5)</f>
+      <c r="D35" s="1">
+        <f>1.1 *$A$1 * IF(A35 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
-      <c r="F34" s="1">
+      <c r="E35" s="1">
         <f t="shared" si="0"/>
         <v>1247.4000000000001</v>
       </c>
-      <c r="G34" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H34" s="3">
+      <c r="F35" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G35" s="3">
         <f t="shared" si="6"/>
         <v>44837</v>
       </c>
-      <c r="I34" s="1">
+      <c r="H35" s="1">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="J34" s="1">
-        <v>10</v>
-      </c>
-      <c r="K34" s="1">
+      <c r="I35" s="1">
+        <v>10</v>
+      </c>
+      <c r="J35" s="1">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="L34" s="1">
+      <c r="K35" s="1">
         <f t="shared" si="2"/>
         <v>1487.4</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="15.75">
-      <c r="B35" s="2">
+    <row r="36" spans="1:11" ht="15.75">
+      <c r="A36" s="2">
         <f t="shared" si="8"/>
         <v>34</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="6">
+      <c r="C36" s="6">
         <f t="shared" si="4"/>
         <v>53.5</v>
       </c>
-      <c r="E35" s="1">
-        <f>1.1 *$A$1 * IF(B35 &lt;= 8*4, 1, 0.5)</f>
+      <c r="D36" s="1">
+        <f>1.1 *$A$1 * IF(A36 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
-      <c r="F35" s="1">
+      <c r="E36" s="1">
         <f t="shared" si="0"/>
         <v>1235.8500000000001</v>
       </c>
-      <c r="G35" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H35" s="3">
+      <c r="F36" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G36" s="3">
         <f t="shared" si="6"/>
         <v>44838</v>
       </c>
-      <c r="I35" s="1">
+      <c r="H36" s="1">
         <f t="shared" si="7"/>
         <v>25</v>
       </c>
-      <c r="J35" s="1">
-        <v>10</v>
-      </c>
-      <c r="K35" s="1">
+      <c r="I36" s="1">
+        <v>10</v>
+      </c>
+      <c r="J36" s="1">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="L35" s="1">
+      <c r="K36" s="1">
         <f t="shared" si="2"/>
         <v>1485.8500000000001</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="15.75">
-      <c r="B36" s="2">
+    <row r="37" spans="1:11" ht="15.75">
+      <c r="A37" s="2">
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="6">
+      <c r="C37" s="6">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="E36" s="1">
-        <f>1.1 *$A$1 * IF(B36 &lt;= 8*4, 1, 0.5)</f>
+      <c r="D37" s="1">
+        <f>1.1 *$A$1 * IF(A37 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
-      <c r="F36" s="1">
+      <c r="E37" s="1">
         <f t="shared" si="0"/>
         <v>1224.3000000000002</v>
       </c>
-      <c r="G36" s="3">
-        <f>$G$2</f>
-        <v>44813</v>
-      </c>
-      <c r="H36" s="3">
+      <c r="F37" s="3">
+        <f>$F$3</f>
+        <v>44813</v>
+      </c>
+      <c r="G37" s="3">
         <f t="shared" si="6"/>
         <v>44839</v>
       </c>
-      <c r="I36" s="1">
+      <c r="H37" s="1">
         <f t="shared" si="7"/>
         <v>26</v>
       </c>
-      <c r="J36" s="1">
-        <v>10</v>
-      </c>
-      <c r="K36" s="1">
+      <c r="I37" s="1">
+        <v>10</v>
+      </c>
+      <c r="J37" s="1">
         <f t="shared" si="1"/>
         <v>260</v>
       </c>
-      <c r="L36" s="1">
+      <c r="K37" s="1">
         <f t="shared" si="2"/>
         <v>1484.3000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="15.75">
-      <c r="B37" s="2">
+    <row r="38" spans="1:11" ht="15.75">
+      <c r="A38" s="2">
         <f t="shared" si="8"/>
         <v>36</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="B38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="6">
+      <c r="C38" s="6">
         <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
-      <c r="E37" s="1">
-        <f>1.1 *$A$1 * IF(B37 &lt;= 8*4, 1, 0.5)</f>
+      <c r="D38" s="1">
+        <f>1.1 *$A$1 * IF(A38 &lt;= 8*4, 1, 0.5)</f>
         <v>23.1</v>
       </c>
-      <c r="F37" s="1">
+      <c r="E38" s="1">
         <f t="shared" si="0"/>
         <v>1212.75</v>
       </c>
-      <c r="G37" s="3">
-        <f t="shared" si="5"/>
-        <v>44813</v>
-      </c>
-      <c r="H37" s="3">
+      <c r="F38" s="3">
+        <f t="shared" si="5"/>
+        <v>44813</v>
+      </c>
+      <c r="G38" s="3">
         <f t="shared" si="6"/>
         <v>44840</v>
       </c>
-      <c r="I37" s="1">
+      <c r="H38" s="1">
         <f t="shared" si="7"/>
         <v>27</v>
       </c>
-      <c r="J37" s="1">
-        <v>10</v>
-      </c>
-      <c r="K37" s="1">
+      <c r="I38" s="1">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1">
         <f t="shared" si="1"/>
         <v>270</v>
       </c>
-      <c r="L37" s="1">
+      <c r="K38" s="1">
         <f t="shared" si="2"/>
         <v>1482.75</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="15.75">
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="2:12" ht="15.75"/>
-    <row r="40" spans="2:12" ht="15.75">
-      <c r="B40" s="4" t="s">
+    <row r="39" spans="1:11" ht="15.75">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75"/>
+    <row r="41" spans="1:11" ht="15.75">
+      <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="4">
-        <f>SUM(L2:L37)</f>
+      <c r="B41" s="4">
+        <f>SUM(K3:K38)</f>
         <v>100730.7</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="2:12" ht="15.75">
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75">
+      <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="1">
-        <f>AVERAGE(D2:D37)</f>
+      <c r="B42" s="1">
+        <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="15.75">
-      <c r="B42" s="1" t="s">
+    <row r="43" spans="1:11" ht="15.75">
+      <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="1">
-        <f>MAX(I2:I37)</f>
+      <c r="B43" s="1">
+        <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="15.75">
-      <c r="B43" s="1" t="s">
+    <row r="44" spans="1:11" ht="15.75">
+      <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="1">
-        <f>MAX(F2:F37)</f>
+      <c r="B44" s="1">
+        <f>MAX(E3:E38)</f>
         <v>3234</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="15.75"/>
-    <row r="45" spans="2:12" ht="15.75"/>
-    <row r="46" spans="2:12" ht="15.75"/>
-    <row r="47" spans="2:12" ht="15.75"/>
-    <row r="48" spans="2:12" ht="15.75"/>
+    <row r="45" spans="1:11" ht="15.75"/>
+    <row r="46" spans="1:11" ht="15.75"/>
+    <row r="47" spans="1:11" ht="15.75"/>
+    <row r="48" spans="1:11" ht="15.75"/>
     <row r="49" ht="15.75"/>
     <row r="50" ht="15.75"/>
     <row r="51" ht="15.75"/>
@@ -2262,6 +2262,7 @@
     <row r="57" ht="15.75"/>
     <row r="58" ht="15.75"/>
     <row r="59" ht="15.75"/>
+    <row r="60" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
attempt fix lab3 4
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8256902-27B3-4001-8697-910CB4052642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{604A3B6D-EAD9-4D99-828B-845BFED732C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,16 +171,16 @@
     <t>Куропаткин 2</t>
   </si>
   <si>
-    <t>общая сумма графы “Итого”, руб</t>
-  </si>
-  <si>
-    <t>средняя площадь, руб./кв.м.</t>
-  </si>
-  <si>
-    <t>максимальный срок просрочки, дней</t>
-  </si>
-  <si>
-    <t>максимальная сумма к оплате, руб.</t>
+    <t>Общая сумма графы “Итого”, руб.</t>
+  </si>
+  <si>
+    <t>Средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>Максимальный срок просрочки, дней</t>
+  </si>
+  <si>
+    <t>Максимальная сумма к оплате, руб.</t>
   </si>
 </sst>
 </file>
@@ -566,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -637,7 +637,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="1">
-        <f>1.1 *$A$1 * IF(A3 &lt;= 8*4, 1, 0.5)</f>
+        <f>$A$1 * IF(A3 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E3" s="1">
@@ -679,11 +679,11 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
-        <f>1.1 *$A$1 * IF(A4 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" ref="D4:D38" si="0">$A$1 * IF(A4 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E38" si="0">C4 * D4</f>
+        <f t="shared" ref="E4:E38" si="1">C4 * D4</f>
         <v>3210.9</v>
       </c>
       <c r="F4" s="3">
@@ -702,1224 +702,1224 @@
         <v>10</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J38" si="1">H4*I4</f>
+        <f t="shared" ref="J4:J38" si="2">H4*I4</f>
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K39" si="2">E4+J4</f>
+        <f t="shared" ref="K4:K39" si="3">E4+J4</f>
         <v>3210.9</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A8" si="3">A4+1</f>
+        <f t="shared" ref="A5:A8" si="4">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" ref="C5:C38" si="4">C4 - 0.5</f>
+        <f t="shared" ref="C5:C38" si="5">C4 - 0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f>1.1 *$A$1 * IF(A5 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3187.8</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F38" si="5">$F$3</f>
+        <f t="shared" ref="F5:F38" si="6">$F$3</f>
         <v>44813</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G38" si="6">G4 + 1</f>
+        <f t="shared" ref="G5:G38" si="7">G4 + 1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H4:H38" si="7">IF(G5 &lt; F5, 0, G5 - F5)</f>
+        <f t="shared" ref="H4:H38" si="8">IF(G5 &lt; F5, 0, G5 - F5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>10</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3187.8</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
-        <f>1.1 *$A$1 * IF(A6 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3164.7000000000003</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44808</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>10</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3164.7000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
       <c r="D7" s="1">
-        <f>1.1 *$A$1 * IF(A7 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3141.6000000000004</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44809</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I7" s="1">
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3141.6000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75">
       <c r="A8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
-        <f>1.1 *$A$1 * IF(A8 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3118.5</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44810</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
         <v>10</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3118.5</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75">
       <c r="A9" s="2">
-        <f t="shared" ref="A7:A38" si="8">A8+1</f>
+        <f t="shared" ref="A7:A38" si="9">A8+1</f>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <f>1.1 *$A$1 * IF(A9 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3095.4</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44811</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I9" s="1">
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3095.4</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75">
       <c r="A10" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
-        <f>1.1 *$A$1 * IF(A10 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3072.3</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44812</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I10" s="1">
         <v>10</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3072.3</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="D11" s="1">
-        <f>1.1 *$A$1 * IF(A11 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3049.2000000000003</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I11" s="1">
         <v>10</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3049.2000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75">
       <c r="A12" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
-        <f>1.1 *$A$1 * IF(A12 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3026.1000000000004</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44814</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I12" s="1">
         <v>10</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3036.1000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <f>1.1 *$A$1 * IF(A13 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3003</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44815</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="I13" s="1">
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3023</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
-        <f>1.1 *$A$1 * IF(A14 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2979.9</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I14" s="1">
         <v>10</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3009.9</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="D15" s="1">
-        <f>1.1 *$A$1 * IF(A15 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2956.8</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44817</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="I15" s="1">
         <v>10</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2996.8</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
-        <f>1.1 *$A$1 * IF(A16 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2933.7000000000003</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44818</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="I16" s="1">
         <v>10</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2983.7000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75">
       <c r="A17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="D17" s="1">
-        <f>1.1 *$A$1 * IF(A17 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2910.6000000000004</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44819</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="I17" s="1">
         <v>10</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2970.6000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
-        <f>1.1 *$A$1 * IF(A18 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2887.5</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44820</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="I18" s="1">
         <v>10</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2957.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62</v>
       </c>
       <c r="D19" s="1">
-        <f>1.1 *$A$1 * IF(A19 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2864.4</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44821</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="I19" s="1">
         <v>10</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2944.4</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75">
       <c r="A20" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
-        <f>1.1 *$A$1 * IF(A20 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2841.3</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44822</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="I20" s="1">
         <v>10</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2931.3</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75">
       <c r="A21" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f>1.1 *$A$1 * IF(A21 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2818.2000000000003</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44823</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="I21" s="1">
         <v>10</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2918.2000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75">
       <c r="A22" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
-        <f>1.1 *$A$1 * IF(A22 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2795.1000000000004</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44824</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="I22" s="1">
         <v>10</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2905.1000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75">
       <c r="A23" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f>1.1 *$A$1 * IF(A23 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2772</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44825</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="I23" s="1">
         <v>10</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2892</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75">
       <c r="A24" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
-        <f>1.1 *$A$1 * IF(A24 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2748.9</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44826</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="I24" s="1">
         <v>10</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2878.9</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75">
       <c r="A25" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f>1.1 *$A$1 * IF(A25 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.8</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44827</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="I25" s="1">
         <v>10</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2865.8</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75">
       <c r="A26" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
-        <f>1.1 *$A$1 * IF(A26 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2702.7000000000003</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44828</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="I26" s="1">
         <v>10</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2852.7000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75">
       <c r="A27" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="D27" s="1">
-        <f>1.1 *$A$1 * IF(A27 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2679.6000000000004</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44829</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="I27" s="1">
         <v>10</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2839.6000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75">
       <c r="A28" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
-        <f>1.1 *$A$1 * IF(A28 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2656.5</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44830</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="I28" s="1">
         <v>10</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2826.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57</v>
       </c>
       <c r="D29" s="1">
-        <f>1.1 *$A$1 * IF(A29 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2633.4</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44831</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="I29" s="1">
         <v>10</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2813.4</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75">
       <c r="A30" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
-        <f>1.1 *$A$1 * IF(A30 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2610.3000000000002</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44832</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="I30" s="1">
         <v>10</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2800.3</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75">
       <c r="A31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="D31" s="1">
-        <f>1.1 *$A$1 * IF(A31 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2587.2000000000003</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44833</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="I31" s="1">
         <v>10</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2787.2000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
-        <f>1.1 *$A$1 * IF(A32 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2564.1000000000004</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G32" s="3">
@@ -1927,215 +1927,215 @@
         <v>44834</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="I32" s="1">
         <v>10</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2774.1000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75">
       <c r="A33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="D33" s="1">
-        <f>1.1 *$A$1 * IF(A33 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2541</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44835</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="I33" s="1">
         <v>10</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2761</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75">
       <c r="A34" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
-        <f>1.1 *$A$1 * IF(A34 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2517.9</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44836</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="I34" s="1">
         <v>10</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>230</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2747.9</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75">
       <c r="A35" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>1.1 *$A$1 * IF(A35 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>23.1</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1247.4000000000001</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44837</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="I35" s="1">
         <v>10</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1487.4</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75">
       <c r="A36" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C36" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f>1.1 *$A$1 * IF(A36 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>23.1</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1235.8500000000001</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44838</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="I36" s="1">
         <v>10</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1485.8500000000001</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75">
       <c r="A37" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f>1.1 *$A$1 * IF(A37 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>23.1</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1224.3000000000002</v>
       </c>
       <c r="F37" s="3">
@@ -2143,110 +2143,109 @@
         <v>44813</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44839</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="I37" s="1">
         <v>10</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1484.3000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75">
       <c r="A38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C38" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f>1.1 *$A$1 * IF(A38 &lt;= 8*4, 1, 0.5)</f>
+        <f t="shared" si="0"/>
         <v>23.1</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1212.75</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44813</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44840</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="I38" s="1">
         <v>10</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1482.75</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75">
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75"/>
-    <row r="41" spans="1:11" ht="15.75">
-      <c r="A41" s="4" t="s">
+    <row r="40" spans="1:11" ht="15.75">
+      <c r="B40" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="4">
+      <c r="C40" s="4">
         <f>SUM(K3:K38)</f>
         <v>100730.7</v>
       </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="41" spans="1:11" ht="15.75">
+      <c r="B41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="1">
+      <c r="C41" s="1">
         <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75">
-      <c r="A43" s="1" t="s">
+    <row r="42" spans="1:11" ht="15.75">
+      <c r="B42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C42" s="1">
         <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75">
-      <c r="A44" s="1" t="s">
+    <row r="43" spans="1:11" ht="15.75">
+      <c r="B43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="1">
+      <c r="C43" s="1">
         <f>MAX(E3:E38)</f>
         <v>3234</v>
       </c>
     </row>
+    <row r="44" spans="1:11" ht="15.75"/>
     <row r="45" spans="1:11" ht="15.75"/>
     <row r="46" spans="1:11" ht="15.75"/>
     <row r="47" spans="1:11" ht="15.75"/>
@@ -2263,6 +2262,7 @@
     <row r="58" ht="15.75"/>
     <row r="59" ht="15.75"/>
     <row r="60" ht="15.75"/>
+    <row r="61" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
attempt fix lab3 5
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{604A3B6D-EAD9-4D99-828B-845BFED732C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03971FF0-F70F-4189-8A61-407110A7669C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
     <t>Куропаткин 2</t>
   </si>
   <si>
-    <t>Общая сумма графы “Итого”, руб.</t>
+    <t>Общая сумма графы, руб.</t>
   </si>
   <si>
     <t>Средняя площадь, кв.м.</t>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2241,7 +2241,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="1">
-        <f>MAX(E3:E38)</f>
+        <f>MAX(K3:K38)</f>
         <v>3234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
attempt fix lab3 7
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47FF8DC7-199A-4B9E-94F6-18793C7D1E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1E3C8EF-7FC1-4960-A5D4-75AA05D9CF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FA2EC11-4BA8-4080-A836-9909C04E522C}"/>
   </bookViews>
@@ -179,16 +179,16 @@
     <t>Куропаткин 2</t>
   </si>
   <si>
-    <t>Общая сумма, руб.</t>
-  </si>
-  <si>
-    <t>Средняя площадь, кв.м.</t>
-  </si>
-  <si>
-    <t>Максимальный срок просрочки, дней</t>
-  </si>
-  <si>
-    <t>Максимальная сумма к оплате, руб.</t>
+    <t>общая сумма, руб.</t>
+  </si>
+  <si>
+    <t>средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>максимальный срок просрочки, дней</t>
+  </si>
+  <si>
+    <t>максимальная сумма к оплате, руб.</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEDB43A-7E00-4476-B32F-89C95E40AD8A}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2120,7 +2120,7 @@
         <v>100730.7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="31.5">
+    <row r="41" spans="1:11">
       <c r="B41" s="6" t="s">
         <v>48</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>61.25</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="31.5">
+    <row r="42" spans="1:11" ht="30.75">
       <c r="B42" s="6" t="s">
         <v>49</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="31.5">
+    <row r="43" spans="1:11" ht="30.75">
       <c r="B43" s="6" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
attempt fix lab3 8
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1E3C8EF-7FC1-4960-A5D4-75AA05D9CF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE8010C4-9F81-4F05-9076-397308DA86B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FA2EC11-4BA8-4080-A836-9909C04E522C}"/>
   </bookViews>
@@ -65,7 +65,7 @@
     <t>Пени за 1 день</t>
   </si>
   <si>
-    <t>Штраф, руб</t>
+    <t>Штраф, руб.</t>
   </si>
   <si>
     <t>Итого, руб.</t>
@@ -179,16 +179,16 @@
     <t>Куропаткин 2</t>
   </si>
   <si>
-    <t>общая сумма, руб.</t>
-  </si>
-  <si>
-    <t>средняя площадь, кв.м.</t>
-  </si>
-  <si>
-    <t>максимальный срок просрочки, дней</t>
-  </si>
-  <si>
-    <t>максимальная сумма к оплате, руб.</t>
+    <t>Общая сумма, руб.</t>
+  </si>
+  <si>
+    <t>Средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>Максимальный срок просрочки, дней</t>
+  </si>
+  <si>
+    <t>Максимальная сумма к оплате, руб.</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEDB43A-7E00-4476-B32F-89C95E40AD8A}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
attempt fix lab3 9
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE8010C4-9F81-4F05-9076-397308DA86B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E64AABA8-F37B-4C39-8C48-E5D0319472FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FA2EC11-4BA8-4080-A836-9909C04E522C}"/>
   </bookViews>
@@ -179,16 +179,16 @@
     <t>Куропаткин 2</t>
   </si>
   <si>
-    <t>Общая сумма, руб.</t>
-  </si>
-  <si>
-    <t>Средняя площадь, кв.м.</t>
+    <t>Общая сумма, руб</t>
+  </si>
+  <si>
+    <t>Средняя площадь, кв.м</t>
   </si>
   <si>
     <t>Максимальный срок просрочки, дней</t>
   </si>
   <si>
-    <t>Максимальная сумма к оплате, руб.</t>
+    <t>Максимальная сумма к оплате, руб</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEDB43A-7E00-4476-B32F-89C95E40AD8A}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -688,11 +688,11 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D17" si="0" xml:space="preserve"> $A$1 * IF(A4 &lt;= 32, 1.1, 0.55)</f>
+        <f xml:space="preserve"> $A$1 * IF(A4 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E38" si="1">C4 * D4</f>
+        <f t="shared" ref="E4:E38" si="0">C4 * D4</f>
         <v>3210.9</v>
       </c>
       <c r="F4" s="5">
@@ -702,18 +702,18 @@
         <v>44806</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H38" si="2">IF(F4&lt;G4,G4-F4,0)</f>
+        <f t="shared" ref="H4:H38" si="1">IF(F4&lt;G4,G4-F4,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="3">
         <v>10</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J38" si="3">I4 * H4</f>
+        <f t="shared" ref="J4:J38" si="2">I4 * H4</f>
         <v>0</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K38" si="4">J4 + E4</f>
+        <f t="shared" ref="K4:K38" si="3">J4 + E4</f>
         <v>3210.9</v>
       </c>
     </row>
@@ -725,15 +725,15 @@
         <v>13</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
+        <f t="shared" ref="C5:C38" si="4">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A5 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3187.8</v>
       </c>
       <c r="F5" s="5">
@@ -743,18 +743,18 @@
         <v>44807</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="3">
         <v>10</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3187.8</v>
       </c>
     </row>
@@ -766,15 +766,15 @@
         <v>14</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>68.5</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A6 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3164.7000000000003</v>
       </c>
       <c r="F6" s="5">
@@ -784,18 +784,18 @@
         <v>44808</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="3">
         <v>10</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3164.7000000000003</v>
       </c>
     </row>
@@ -807,15 +807,15 @@
         <v>15</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A7 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3141.6000000000004</v>
       </c>
       <c r="F7" s="5">
@@ -825,18 +825,18 @@
         <v>44809</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="3">
         <v>10</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3141.6000000000004</v>
       </c>
     </row>
@@ -848,15 +848,15 @@
         <v>16</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A8 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3118.5</v>
       </c>
       <c r="F8" s="5">
@@ -866,18 +866,18 @@
         <v>44810</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" s="3">
         <v>10</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3118.5</v>
       </c>
     </row>
@@ -889,15 +889,15 @@
         <v>17</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A9 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3095.4</v>
       </c>
       <c r="F9" s="5">
@@ -907,18 +907,18 @@
         <v>44811</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" s="3">
         <v>10</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3095.4</v>
       </c>
     </row>
@@ -930,15 +930,15 @@
         <v>18</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>66.5</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A10 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3072.3</v>
       </c>
       <c r="F10" s="5">
@@ -948,18 +948,18 @@
         <v>44812</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>10</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3072.3</v>
       </c>
     </row>
@@ -971,15 +971,15 @@
         <v>19</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A11 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3049.2000000000003</v>
       </c>
       <c r="F11" s="5">
@@ -989,18 +989,18 @@
         <v>44813</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I11" s="3">
         <v>10</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3049.2000000000003</v>
       </c>
     </row>
@@ -1012,15 +1012,15 @@
         <v>20</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>65.5</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A12 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3026.1000000000004</v>
       </c>
       <c r="F12" s="5">
@@ -1030,18 +1030,18 @@
         <v>44814</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I12" s="3">
         <v>10</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3036.1000000000004</v>
       </c>
     </row>
@@ -1053,15 +1053,15 @@
         <v>21</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A13 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3003</v>
       </c>
       <c r="F13" s="5">
@@ -1071,18 +1071,18 @@
         <v>44815</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I13" s="3">
         <v>10</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3023</v>
       </c>
     </row>
@@ -1094,15 +1094,15 @@
         <v>22</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>64.5</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A14 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2979.9</v>
       </c>
       <c r="F14" s="5">
@@ -1112,18 +1112,18 @@
         <v>44816</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I14" s="3">
         <v>10</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3009.9</v>
       </c>
     </row>
@@ -1135,15 +1135,15 @@
         <v>23</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A15 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2956.8</v>
       </c>
       <c r="F15" s="5">
@@ -1153,18 +1153,18 @@
         <v>44817</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I15" s="3">
         <v>10</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2996.8</v>
       </c>
     </row>
@@ -1176,15 +1176,15 @@
         <v>24</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63.5</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A16 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2933.7000000000003</v>
       </c>
       <c r="F16" s="5">
@@ -1194,18 +1194,18 @@
         <v>44818</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I16" s="3">
         <v>10</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2983.7000000000003</v>
       </c>
     </row>
@@ -1217,15 +1217,15 @@
         <v>25</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> $A$1 * IF(A17 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2910.6000000000004</v>
       </c>
       <c r="F17" s="5">
@@ -1235,18 +1235,18 @@
         <v>44819</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I17" s="3">
         <v>10</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="K17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2970.6000000000004</v>
       </c>
     </row>
@@ -1258,7 +1258,7 @@
         <v>26</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
       <c r="D18" s="3">
@@ -1266,7 +1266,7 @@
         <v>46.2</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2887.5</v>
       </c>
       <c r="F18" s="5">
@@ -1276,18 +1276,18 @@
         <v>44820</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I18" s="3">
         <v>10</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2957.5</v>
       </c>
     </row>
@@ -1299,15 +1299,15 @@
         <v>27</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" ref="D19:D38" si="6" xml:space="preserve"> $A$1 * IF(A19 &lt;= 32, 1.1, 0.55)</f>
+        <f xml:space="preserve"> $A$1 * IF(A19 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2864.4</v>
       </c>
       <c r="F19" s="5">
@@ -1317,18 +1317,18 @@
         <v>44821</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I19" s="3">
         <v>10</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2944.4</v>
       </c>
     </row>
@@ -1340,15 +1340,15 @@
         <v>28</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61.5</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A20 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2841.3</v>
       </c>
       <c r="F20" s="5">
@@ -1358,18 +1358,18 @@
         <v>44822</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="I20" s="3">
         <v>10</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2931.3</v>
       </c>
     </row>
@@ -1381,15 +1381,15 @@
         <v>29</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A21 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2818.2000000000003</v>
       </c>
       <c r="F21" s="5">
@@ -1399,18 +1399,18 @@
         <v>44823</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I21" s="3">
         <v>10</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2918.2000000000003</v>
       </c>
     </row>
@@ -1422,15 +1422,15 @@
         <v>30</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>60.5</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A22 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2795.1000000000004</v>
       </c>
       <c r="F22" s="5">
@@ -1440,18 +1440,18 @@
         <v>44824</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="I22" s="3">
         <v>10</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2905.1000000000004</v>
       </c>
     </row>
@@ -1463,15 +1463,15 @@
         <v>31</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A23 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2772</v>
       </c>
       <c r="F23" s="5">
@@ -1481,18 +1481,18 @@
         <v>44825</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I23" s="3">
         <v>10</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2892</v>
       </c>
     </row>
@@ -1504,15 +1504,15 @@
         <v>32</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>59.5</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A24 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2748.9</v>
       </c>
       <c r="F24" s="5">
@@ -1522,18 +1522,18 @@
         <v>44826</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="I24" s="3">
         <v>10</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2878.9</v>
       </c>
     </row>
@@ -1545,15 +1545,15 @@
         <v>33</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A25 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2725.8</v>
       </c>
       <c r="F25" s="5">
@@ -1563,18 +1563,18 @@
         <v>44827</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="I25" s="3">
         <v>10</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2865.8</v>
       </c>
     </row>
@@ -1586,15 +1586,15 @@
         <v>34</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A26 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2702.7000000000003</v>
       </c>
       <c r="F26" s="5">
@@ -1604,18 +1604,18 @@
         <v>44828</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I26" s="3">
         <v>10</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2852.7000000000003</v>
       </c>
     </row>
@@ -1627,15 +1627,15 @@
         <v>35</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A27 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2679.6000000000004</v>
       </c>
       <c r="F27" s="5">
@@ -1645,18 +1645,18 @@
         <v>44829</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="I27" s="3">
         <v>10</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2839.6000000000004</v>
       </c>
     </row>
@@ -1668,15 +1668,15 @@
         <v>36</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>57.5</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A28 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2656.5</v>
       </c>
       <c r="F28" s="5">
@@ -1686,18 +1686,18 @@
         <v>44830</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="I28" s="3">
         <v>10</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2826.5</v>
       </c>
     </row>
@@ -1709,15 +1709,15 @@
         <v>37</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A29 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2633.4</v>
       </c>
       <c r="F29" s="5">
@@ -1727,18 +1727,18 @@
         <v>44831</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="I29" s="3">
         <v>10</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2813.4</v>
       </c>
     </row>
@@ -1750,15 +1750,15 @@
         <v>38</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>56.5</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A30 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2610.3000000000002</v>
       </c>
       <c r="F30" s="5">
@@ -1768,18 +1768,18 @@
         <v>44832</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="I30" s="3">
         <v>10</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2800.3</v>
       </c>
     </row>
@@ -1791,15 +1791,15 @@
         <v>39</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A31 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2587.2000000000003</v>
       </c>
       <c r="F31" s="5">
@@ -1809,18 +1809,18 @@
         <v>44833</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I31" s="3">
         <v>10</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2787.2000000000003</v>
       </c>
     </row>
@@ -1832,15 +1832,15 @@
         <v>40</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>55.5</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A32 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2564.1000000000004</v>
       </c>
       <c r="F32" s="5">
@@ -1850,18 +1850,18 @@
         <v>44834</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="I32" s="3">
         <v>10</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2774.1000000000004</v>
       </c>
     </row>
@@ -1873,15 +1873,15 @@
         <v>41</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A33 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2541</v>
       </c>
       <c r="F33" s="5">
@@ -1891,18 +1891,18 @@
         <v>44835</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="I33" s="3">
         <v>10</v>
       </c>
       <c r="J33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="K33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2761</v>
       </c>
     </row>
@@ -1914,15 +1914,15 @@
         <v>42</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>54.5</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A34 &lt;= 32, 1.1, 0.55)</f>
         <v>46.2</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2517.9</v>
       </c>
       <c r="F34" s="5">
@@ -1932,18 +1932,18 @@
         <v>44836</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="I34" s="3">
         <v>10</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>230</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2747.9</v>
       </c>
     </row>
@@ -1955,15 +1955,15 @@
         <v>43</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A35 &lt;= 32, 1.1, 0.55)</f>
         <v>23.1</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1247.4000000000001</v>
       </c>
       <c r="F35" s="5">
@@ -1973,18 +1973,18 @@
         <v>44837</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I35" s="3">
         <v>10</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1487.4</v>
       </c>
     </row>
@@ -1996,15 +1996,15 @@
         <v>44</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>53.5</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A36 &lt;= 32, 1.1, 0.55)</f>
         <v>23.1</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1235.8500000000001</v>
       </c>
       <c r="F36" s="5">
@@ -2014,18 +2014,18 @@
         <v>44838</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="I36" s="3">
         <v>10</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1485.8500000000001</v>
       </c>
     </row>
@@ -2037,15 +2037,15 @@
         <v>45</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A37 &lt;= 32, 1.1, 0.55)</f>
         <v>23.1</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1224.3000000000002</v>
       </c>
       <c r="F37" s="5">
@@ -2055,18 +2055,18 @@
         <v>44839</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="I37" s="3">
         <v>10</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1484.3000000000002</v>
       </c>
     </row>
@@ -2078,15 +2078,15 @@
         <v>46</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> $A$1 * IF(A38 &lt;= 32, 1.1, 0.55)</f>
         <v>23.1</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1212.75</v>
       </c>
       <c r="F38" s="5">
@@ -2096,18 +2096,18 @@
         <v>44840</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="I38" s="3">
         <v>10</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1482.75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lab3 final final fix
</commit_message>
<xml_diff>
--- a/LR3/table_1_42.xlsx
+++ b/LR3/table_1_42.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{786164F6-FA52-45BD-8083-FFC307FB7414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E2F33AD-5C23-4466-A4F4-19D439C48D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FA2EC11-4BA8-4080-A836-9909C04E522C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>№ квартиры</t>
   </si>
   <si>
-    <t>Фамилия квартиросъемщика</t>
+    <t>Фамилия квартиросъёмщика</t>
   </si>
   <si>
     <t>Площадь, кв.м.</t>
@@ -173,13 +173,13 @@
     <t>Мохамед</t>
   </si>
   <si>
-    <t>Куропаткин 1</t>
+    <t>Баницин</t>
   </si>
   <si>
     <t>Куропаткин 2</t>
   </si>
   <si>
-    <t>Общая сумма графы "Итого", руб.</t>
+    <t>Общая сумма, руб.</t>
   </si>
   <si>
     <t>Средняя площадь, кв.м.</t>
@@ -576,14 +576,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEDB43A-7E00-4476-B32F-89C95E40AD8A}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.125" style="6" customWidth="1"/>
     <col min="3" max="3" width="14" style="3" customWidth="1"/>
     <col min="4" max="4" width="17" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.875" style="3" customWidth="1"/>
@@ -2111,7 +2111,7 @@
         <v>1482.75</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30.75">
+    <row r="40" spans="1:11">
       <c r="B40" s="6" t="s">
         <v>47</v>
       </c>

</xml_diff>